<commit_message>
Factor out more division using mul by reciprocal.
</commit_message>
<xml_diff>
--- a/GBADoomMemory.xlsx
+++ b/GBADoomMemory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\GBADoom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58763E81-8346-4A79-A960-34C49D0C0FE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A5B7A3-8677-44C1-A174-B459518F1EA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7230" yWindow="3600" windowWidth="21570" windowHeight="11370" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7230" yWindow="480" windowWidth="21570" windowHeight="11370" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="1" r:id="rId1"/>
@@ -34,18 +34,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="285">
   <si>
     <t>Memory</t>
   </si>
@@ -895,6 +889,12 @@
   <si>
     <t>group lines</t>
   </si>
+  <si>
+    <t>RDiv1</t>
+  </si>
+  <si>
+    <t>RDiv2</t>
+  </si>
 </sst>
 </file>
 
@@ -960,7 +960,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -976,6 +976,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14533,7 +14534,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16316,15 +16317,16 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A2:Q278"/>
+  <dimension ref="A2:Q284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="I268" sqref="I268"/>
+    <sheetView topLeftCell="A268" workbookViewId="0">
+      <selection activeCell="F284" sqref="F283:F284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
@@ -19122,7 +19124,7 @@
         <v>1.018987341772152</v>
       </c>
     </row>
-    <row r="274" spans="1:3">
+    <row r="274" spans="1:11">
       <c r="A274">
         <v>124210</v>
       </c>
@@ -19134,7 +19136,7 @@
         <v>0.23705015699219065</v>
       </c>
     </row>
-    <row r="275" spans="1:3">
+    <row r="275" spans="1:11">
       <c r="A275">
         <v>742611</v>
       </c>
@@ -19145,8 +19147,9 @@
         <f>B275/A275</f>
         <v>0.2756207489520085</v>
       </c>
-    </row>
-    <row r="276" spans="1:3">
+      <c r="K275" s="1"/>
+    </row>
+    <row r="276" spans="1:11">
       <c r="A276">
         <v>457391</v>
       </c>
@@ -19157,8 +19160,9 @@
         <f>B276/A276</f>
         <v>0.32211390254727357</v>
       </c>
-    </row>
-    <row r="277" spans="1:3">
+      <c r="K276" s="1"/>
+    </row>
+    <row r="277" spans="1:11">
       <c r="A277">
         <v>891854</v>
       </c>
@@ -19169,8 +19173,9 @@
         <f>B277/A277</f>
         <v>0.33953203102750001</v>
       </c>
-    </row>
-    <row r="278" spans="1:3">
+      <c r="K277" s="1"/>
+    </row>
+    <row r="278" spans="1:11">
       <c r="A278">
         <v>700363</v>
       </c>
@@ -19181,6 +19186,36 @@
         <f>B278/A278</f>
         <v>0.50375162594254697</v>
       </c>
+      <c r="K278" s="1"/>
+    </row>
+    <row r="279" spans="1:11">
+      <c r="K279" s="1"/>
+    </row>
+    <row r="282" spans="1:11">
+      <c r="A282" t="s">
+        <v>283</v>
+      </c>
+      <c r="B282">
+        <v>23</v>
+      </c>
+      <c r="C282" s="13">
+        <v>362609</v>
+      </c>
+    </row>
+    <row r="283" spans="1:11">
+      <c r="A283" t="s">
+        <v>284</v>
+      </c>
+      <c r="C283" s="13">
+        <v>398478</v>
+      </c>
+      <c r="D283" s="1">
+        <f>C283/C282</f>
+        <v>1.0989192215306294</v>
+      </c>
+    </row>
+    <row r="284" spans="1:11">
+      <c r="C284" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -25870,8 +25905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28243,6 +28278,162 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0600-000001000000}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J2:J2</xm:f>
+              <xm:sqref>K2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J3:J3</xm:f>
+              <xm:sqref>K3</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J4:J4</xm:f>
+              <xm:sqref>K4</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J5:J5</xm:f>
+              <xm:sqref>K5</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J6:J6</xm:f>
+              <xm:sqref>K6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J7:J7</xm:f>
+              <xm:sqref>K7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J8:J8</xm:f>
+              <xm:sqref>K8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J9:J9</xm:f>
+              <xm:sqref>K9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J10:J10</xm:f>
+              <xm:sqref>K10</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J11:J11</xm:f>
+              <xm:sqref>K11</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J12:J12</xm:f>
+              <xm:sqref>K12</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J13:J13</xm:f>
+              <xm:sqref>K13</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J14:J14</xm:f>
+              <xm:sqref>K14</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J15:J15</xm:f>
+              <xm:sqref>K15</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J16:J16</xm:f>
+              <xm:sqref>K16</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J17:J17</xm:f>
+              <xm:sqref>K17</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J18:J18</xm:f>
+              <xm:sqref>K18</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J19:J19</xm:f>
+              <xm:sqref>K19</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J20:J20</xm:f>
+              <xm:sqref>K20</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J21:J21</xm:f>
+              <xm:sqref>K21</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J22:J22</xm:f>
+              <xm:sqref>K22</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J23:J23</xm:f>
+              <xm:sqref>K23</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J24:J24</xm:f>
+              <xm:sqref>K24</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J25:J25</xm:f>
+              <xm:sqref>K25</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J26:J26</xm:f>
+              <xm:sqref>K26</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J27:J27</xm:f>
+              <xm:sqref>K27</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J28:J28</xm:f>
+              <xm:sqref>K28</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J29:J29</xm:f>
+              <xm:sqref>K29</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J30:J30</xm:f>
+              <xm:sqref>K30</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J31:J31</xm:f>
+              <xm:sqref>K31</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J32:J32</xm:f>
+              <xm:sqref>K32</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J33:J33</xm:f>
+              <xm:sqref>K33</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J34:J34</xm:f>
+              <xm:sqref>K34</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J35:J35</xm:f>
+              <xm:sqref>K35</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J36:J36</xm:f>
+              <xm:sqref>K36</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J37:J37</xm:f>
+              <xm:sqref>K37</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0600-000000000000}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
@@ -28399,162 +28590,6 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0600-000001000000}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J2:J2</xm:f>
-              <xm:sqref>K2</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J3:J3</xm:f>
-              <xm:sqref>K3</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J4:J4</xm:f>
-              <xm:sqref>K4</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J5:J5</xm:f>
-              <xm:sqref>K5</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J6:J6</xm:f>
-              <xm:sqref>K6</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J7:J7</xm:f>
-              <xm:sqref>K7</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J8:J8</xm:f>
-              <xm:sqref>K8</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J9:J9</xm:f>
-              <xm:sqref>K9</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J10:J10</xm:f>
-              <xm:sqref>K10</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J11:J11</xm:f>
-              <xm:sqref>K11</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J12:J12</xm:f>
-              <xm:sqref>K12</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J13:J13</xm:f>
-              <xm:sqref>K13</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J14:J14</xm:f>
-              <xm:sqref>K14</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J15:J15</xm:f>
-              <xm:sqref>K15</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J16:J16</xm:f>
-              <xm:sqref>K16</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J17:J17</xm:f>
-              <xm:sqref>K17</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J18:J18</xm:f>
-              <xm:sqref>K18</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J19:J19</xm:f>
-              <xm:sqref>K19</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J20:J20</xm:f>
-              <xm:sqref>K20</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J21:J21</xm:f>
-              <xm:sqref>K21</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J22:J22</xm:f>
-              <xm:sqref>K22</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J23:J23</xm:f>
-              <xm:sqref>K23</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J24:J24</xm:f>
-              <xm:sqref>K24</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J25:J25</xm:f>
-              <xm:sqref>K25</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J26:J26</xm:f>
-              <xm:sqref>K26</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J27:J27</xm:f>
-              <xm:sqref>K27</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J28:J28</xm:f>
-              <xm:sqref>K28</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J29:J29</xm:f>
-              <xm:sqref>K29</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J30:J30</xm:f>
-              <xm:sqref>K30</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J31:J31</xm:f>
-              <xm:sqref>K31</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J32:J32</xm:f>
-              <xm:sqref>K32</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J33:J33</xm:f>
-              <xm:sqref>K33</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J34:J34</xm:f>
-              <xm:sqref>K34</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J35:J35</xm:f>
-              <xm:sqref>K35</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J36:J36</xm:f>
-              <xm:sqref>K36</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J37:J37</xm:f>
-              <xm:sqref>K37</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>
@@ -30559,7 +30594,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0700-000002000000}">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{D21CAF72-2AF7-4E10-80D4-49E1123EB21E}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -30570,8 +30605,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Doom2 Levels'!G2:G2</xm:f>
-              <xm:sqref>H2</xm:sqref>
+              <xm:f>'Doom2 Levels'!L2:L2</xm:f>
+              <xm:sqref>M2</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -30591,7 +30626,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{D21CAF72-2AF7-4E10-80D4-49E1123EB21E}">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0700-000002000000}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -30602,8 +30637,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Doom2 Levels'!L2:L2</xm:f>
-              <xm:sqref>M2</xm:sqref>
+              <xm:f>'Doom2 Levels'!G2:G2</xm:f>
+              <xm:sqref>H2</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>

<commit_message>
Try out msvc ASAN
</commit_message>
<xml_diff>
--- a/GBADoomMemory.xlsx
+++ b/GBADoomMemory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\GBADoom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B706AF-D9A1-41DF-9816-503F80E0271F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D500E6-1CB9-41BC-B98E-0721B0E02A9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="1" r:id="rId1"/>
@@ -13374,8 +13374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14555,7 +14555,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16340,8 +16340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A2:Q291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="A292" sqref="A292"/>
+    <sheetView topLeftCell="A274" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100:XFD100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20118,8 +20118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20961,8 +20961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22260,7 +22260,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23365,8 +23365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:XFD58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24059,8 +24059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -26010,8 +26010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28383,6 +28383,162 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0600-000001000000}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J2:J2</xm:f>
+              <xm:sqref>K2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J3:J3</xm:f>
+              <xm:sqref>K3</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J4:J4</xm:f>
+              <xm:sqref>K4</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J5:J5</xm:f>
+              <xm:sqref>K5</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J6:J6</xm:f>
+              <xm:sqref>K6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J7:J7</xm:f>
+              <xm:sqref>K7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J8:J8</xm:f>
+              <xm:sqref>K8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J9:J9</xm:f>
+              <xm:sqref>K9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J10:J10</xm:f>
+              <xm:sqref>K10</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J11:J11</xm:f>
+              <xm:sqref>K11</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J12:J12</xm:f>
+              <xm:sqref>K12</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J13:J13</xm:f>
+              <xm:sqref>K13</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J14:J14</xm:f>
+              <xm:sqref>K14</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J15:J15</xm:f>
+              <xm:sqref>K15</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J16:J16</xm:f>
+              <xm:sqref>K16</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J17:J17</xm:f>
+              <xm:sqref>K17</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J18:J18</xm:f>
+              <xm:sqref>K18</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J19:J19</xm:f>
+              <xm:sqref>K19</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J20:J20</xm:f>
+              <xm:sqref>K20</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J21:J21</xm:f>
+              <xm:sqref>K21</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J22:J22</xm:f>
+              <xm:sqref>K22</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J23:J23</xm:f>
+              <xm:sqref>K23</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J24:J24</xm:f>
+              <xm:sqref>K24</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J25:J25</xm:f>
+              <xm:sqref>K25</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J26:J26</xm:f>
+              <xm:sqref>K26</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J27:J27</xm:f>
+              <xm:sqref>K27</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J28:J28</xm:f>
+              <xm:sqref>K28</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J29:J29</xm:f>
+              <xm:sqref>K29</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J30:J30</xm:f>
+              <xm:sqref>K30</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J31:J31</xm:f>
+              <xm:sqref>K31</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J32:J32</xm:f>
+              <xm:sqref>K32</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J33:J33</xm:f>
+              <xm:sqref>K33</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J34:J34</xm:f>
+              <xm:sqref>K34</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J35:J35</xm:f>
+              <xm:sqref>K35</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J36:J36</xm:f>
+              <xm:sqref>K36</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J37:J37</xm:f>
+              <xm:sqref>K37</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0600-000000000000}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
@@ -28539,162 +28695,6 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0600-000001000000}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J2:J2</xm:f>
-              <xm:sqref>K2</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J3:J3</xm:f>
-              <xm:sqref>K3</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J4:J4</xm:f>
-              <xm:sqref>K4</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J5:J5</xm:f>
-              <xm:sqref>K5</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J6:J6</xm:f>
-              <xm:sqref>K6</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J7:J7</xm:f>
-              <xm:sqref>K7</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J8:J8</xm:f>
-              <xm:sqref>K8</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J9:J9</xm:f>
-              <xm:sqref>K9</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J10:J10</xm:f>
-              <xm:sqref>K10</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J11:J11</xm:f>
-              <xm:sqref>K11</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J12:J12</xm:f>
-              <xm:sqref>K12</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J13:J13</xm:f>
-              <xm:sqref>K13</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J14:J14</xm:f>
-              <xm:sqref>K14</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J15:J15</xm:f>
-              <xm:sqref>K15</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J16:J16</xm:f>
-              <xm:sqref>K16</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J17:J17</xm:f>
-              <xm:sqref>K17</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J18:J18</xm:f>
-              <xm:sqref>K18</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J19:J19</xm:f>
-              <xm:sqref>K19</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J20:J20</xm:f>
-              <xm:sqref>K20</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J21:J21</xm:f>
-              <xm:sqref>K21</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J22:J22</xm:f>
-              <xm:sqref>K22</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J23:J23</xm:f>
-              <xm:sqref>K23</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J24:J24</xm:f>
-              <xm:sqref>K24</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J25:J25</xm:f>
-              <xm:sqref>K25</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J26:J26</xm:f>
-              <xm:sqref>K26</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J27:J27</xm:f>
-              <xm:sqref>K27</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J28:J28</xm:f>
-              <xm:sqref>K28</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J29:J29</xm:f>
-              <xm:sqref>K29</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J30:J30</xm:f>
-              <xm:sqref>K30</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J31:J31</xm:f>
-              <xm:sqref>K31</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J32:J32</xm:f>
-              <xm:sqref>K32</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J33:J33</xm:f>
-              <xm:sqref>K33</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J34:J34</xm:f>
-              <xm:sqref>K34</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J35:J35</xm:f>
-              <xm:sqref>K35</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J36:J36</xm:f>
-              <xm:sqref>K36</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J37:J37</xm:f>
-              <xm:sqref>K37</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>
@@ -28706,7 +28706,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O31"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30699,7 +30699,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0700-000002000000}">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{D21CAF72-2AF7-4E10-80D4-49E1123EB21E}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -30710,8 +30710,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Doom2 Levels'!G2:G2</xm:f>
-              <xm:sqref>H2</xm:sqref>
+              <xm:f>'Doom2 Levels'!L2:L2</xm:f>
+              <xm:sqref>M2</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -30731,7 +30731,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{D21CAF72-2AF7-4E10-80D4-49E1123EB21E}">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0700-000002000000}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -30742,8 +30742,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Doom2 Levels'!L2:L2</xm:f>
-              <xm:sqref>M2</xm:sqref>
+              <xm:f>'Doom2 Levels'!G2:G2</xm:f>
+              <xm:sqref>H2</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -30757,11 +30757,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E70020B-64A4-492D-9830-6A4BD6B3C292}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C41" sqref="A34:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Add screen wipe segue.
Backported from https://github.com/next-hack/nRF52840Doom
</commit_message>
<xml_diff>
--- a/GBADoomMemory.xlsx
+++ b/GBADoomMemory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\GBADoom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D500E6-1CB9-41BC-B98E-0721B0E02A9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3293F6B-57CB-4F3B-BC91-680564B85BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,19 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="295">
   <si>
     <t>Memory</t>
   </si>
@@ -916,6 +923,15 @@
   <si>
     <t>Rdiv If5</t>
   </si>
+  <si>
+    <t>Trim Zone</t>
+  </si>
+  <si>
+    <t>Zone Trim</t>
+  </si>
+  <si>
+    <t>Mobj trim</t>
+  </si>
 </sst>
 </file>
 
@@ -2776,10 +2792,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>E1M1!$B$2:$B$54</c:f>
+              <c:f>E1M1!$B$2:$B$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="53"/>
+                <c:ptCount val="56"/>
                 <c:pt idx="0">
                   <c:v>572432</c:v>
                 </c:pt>
@@ -2938,6 +2954,15 @@
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>89472</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>89112</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>88752</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>88032</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3397,10 +3422,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>E1M2!$B$2:$B$46</c:f>
+              <c:f>E1M2!$B$2:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>367176</c:v>
                 </c:pt>
@@ -3535,6 +3560,15 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>138664</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>137944</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>137224</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>135784</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4101,109 +4135,109 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>89472</c:v>
+                  <c:v>88032</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>138664</c:v>
+                  <c:v>135784</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>167620</c:v>
+                  <c:v>138600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>134604</c:v>
+                  <c:v>111940</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>133620</c:v>
+                  <c:v>109564</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>197068</c:v>
+                  <c:v>164392</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>154032</c:v>
+                  <c:v>126912</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>103356</c:v>
+                  <c:v>86504</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>129824</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>97796</c:v>
+                  <c:v>78900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>197248</c:v>
+                  <c:v>164800</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>138752</c:v>
+                  <c:v>113988</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>164136</c:v>
+                  <c:v>136888</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>181388</c:v>
+                  <c:v>151832</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>163660</c:v>
+                  <c:v>135492</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>197616</c:v>
+                  <c:v>165864</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>74292</c:v>
+                  <c:v>60808</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>70880</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>80580</c:v>
+                  <c:v>64272</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>113980</c:v>
+                  <c:v>92964</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>151444</c:v>
+                  <c:v>122872</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>168112</c:v>
+                  <c:v>139744</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>183988</c:v>
+                  <c:v>152552</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>156788</c:v>
+                  <c:v>129080</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>136976</c:v>
+                  <c:v>112722</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>68728</c:v>
+                  <c:v>54224</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>119224</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>106076</c:v>
+                  <c:v>85404</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>142768</c:v>
+                  <c:v>117112</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>161720</c:v>
+                  <c:v>134592</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>110740</c:v>
+                  <c:v>89492</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>168980</c:v>
+                  <c:v>140220</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>184264</c:v>
+                  <c:v>152684</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>195892</c:v>
+                  <c:v>162748</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>186336</c:v>
+                  <c:v>153964</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>198756</c:v>
@@ -5554,28 +5588,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>194672</c:v>
+                  <c:v>193056</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>193260</c:v>
+                  <c:v>191532</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>159596</c:v>
+                  <c:v>156940</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>334084</c:v>
+                  <c:v>330172</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>249652</c:v>
+                  <c:v>248084</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>384784</c:v>
+                  <c:v>380064</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>416804</c:v>
+                  <c:v>412212</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>196672</c:v>
+                  <c:v>194480</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13374,7 +13408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
@@ -14554,8 +14588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4DB5C2-1263-4F5F-A356-135B21345C52}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20959,10 +20993,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55:C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20989,15 +21023,15 @@
         <v>572432</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D54" si="0">$F$2-B2</f>
+        <f t="shared" ref="D2:D57" si="0">$F$2-B2</f>
         <v>-310288</v>
       </c>
       <c r="E2" s="1">
-        <f t="shared" ref="E2:E54" si="1">1-(D2/$F$2)</f>
+        <f t="shared" ref="E2:E57" si="1">1-(D2/$F$2)</f>
         <v>2.18365478515625</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F54" si="2">256*1024</f>
+        <f t="shared" ref="F2:F57" si="2">256*1024</f>
         <v>262144</v>
       </c>
     </row>
@@ -21009,7 +21043,7 @@
         <v>533516</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C54" si="3">B2-B3</f>
+        <f t="shared" ref="C3:C57" si="3">B2-B3</f>
         <v>38916</v>
       </c>
       <c r="D3">
@@ -22245,6 +22279,78 @@
         <v>0.34130859375</v>
       </c>
       <c r="F54">
+        <f t="shared" si="2"/>
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>292</v>
+      </c>
+      <c r="B55">
+        <v>89112</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="3"/>
+        <v>360</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>173032</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="1"/>
+        <v>0.339935302734375</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="2"/>
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>294</v>
+      </c>
+      <c r="B56">
+        <v>88752</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="3"/>
+        <v>360</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>173392</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="1"/>
+        <v>0.33856201171875</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="2"/>
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>294</v>
+      </c>
+      <c r="B57">
+        <v>88032</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="3"/>
+        <v>720</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>174112</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="1"/>
+        <v>0.3358154296875</v>
+      </c>
+      <c r="F57">
         <f t="shared" si="2"/>
         <v>262144</v>
       </c>
@@ -22257,10 +22363,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="C47" sqref="C47:C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22287,15 +22393,15 @@
         <v>367176</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D46" si="0">$F$2-B2</f>
+        <f t="shared" ref="D2:D49" si="0">$F$2-B2</f>
         <v>-105032</v>
       </c>
       <c r="E2" s="1">
-        <f t="shared" ref="E2:E46" si="1">1-(D2/$F$2)</f>
+        <f t="shared" ref="E2:E49" si="1">1-(D2/$F$2)</f>
         <v>1.400665283203125</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F46" si="2">256*1024</f>
+        <f t="shared" ref="F2:F49" si="2">256*1024</f>
         <v>262144</v>
       </c>
     </row>
@@ -22931,7 +23037,7 @@
         <v>252316</v>
       </c>
       <c r="C29">
-        <f t="shared" ref="C29:C46" si="4">B28-B29</f>
+        <f t="shared" ref="C29:C49" si="4">B28-B29</f>
         <v>4132</v>
       </c>
       <c r="D29">
@@ -23351,6 +23457,78 @@
         <v>0.528961181640625</v>
       </c>
       <c r="F46">
+        <f t="shared" si="2"/>
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>293</v>
+      </c>
+      <c r="B47">
+        <v>137944</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="4"/>
+        <v>720</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>124200</v>
+      </c>
+      <c r="E47" s="1">
+        <f t="shared" si="1"/>
+        <v>0.526214599609375</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="2"/>
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>294</v>
+      </c>
+      <c r="B48">
+        <v>137224</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="4"/>
+        <v>720</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>124920</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" si="1"/>
+        <v>0.523468017578125</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="2"/>
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>294</v>
+      </c>
+      <c r="B49">
+        <v>135784</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="4"/>
+        <v>1440</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>126360</v>
+      </c>
+      <c r="E49" s="1">
+        <f t="shared" si="1"/>
+        <v>0.517974853515625</v>
+      </c>
+      <c r="F49">
         <f t="shared" si="2"/>
         <v>262144</v>
       </c>
@@ -26010,8 +26188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -26089,15 +26267,15 @@
         <v>85</v>
       </c>
       <c r="B2">
-        <v>89472</v>
+        <v>88032</v>
       </c>
       <c r="C2">
         <f>$E$2-B2</f>
-        <v>172672</v>
+        <v>174112</v>
       </c>
       <c r="D2" s="1">
         <f>1-(C2/$E$2)</f>
-        <v>0.34130859375</v>
+        <v>0.3358154296875</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E37" si="0">256*1024</f>
@@ -26148,15 +26326,15 @@
         <v>86</v>
       </c>
       <c r="B3">
-        <v>138664</v>
+        <v>135784</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C37" si="5">$E$2-B3</f>
-        <v>123480</v>
+        <v>126360</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D37" si="6">1-(C3/$E$2)</f>
-        <v>0.528961181640625</v>
+        <v>0.517974853515625</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
@@ -26207,15 +26385,15 @@
         <v>87</v>
       </c>
       <c r="B4">
-        <v>167620</v>
+        <v>138600</v>
       </c>
       <c r="C4">
         <f t="shared" si="5"/>
-        <v>94524</v>
+        <v>123544</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="6"/>
-        <v>0.6394195556640625</v>
+        <v>0.528717041015625</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
@@ -26266,15 +26444,15 @@
         <v>88</v>
       </c>
       <c r="B5">
-        <v>134604</v>
+        <v>111940</v>
       </c>
       <c r="C5">
         <f t="shared" si="5"/>
-        <v>127540</v>
+        <v>150204</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="6"/>
-        <v>0.5134735107421875</v>
+        <v>0.4270172119140625</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
@@ -26325,15 +26503,15 @@
         <v>89</v>
       </c>
       <c r="B6">
-        <v>133620</v>
+        <v>109564</v>
       </c>
       <c r="C6">
         <f t="shared" si="5"/>
-        <v>128524</v>
+        <v>152580</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="6"/>
-        <v>0.5097198486328125</v>
+        <v>0.4179534912109375</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
@@ -26384,15 +26562,15 @@
         <v>90</v>
       </c>
       <c r="B7">
-        <v>197068</v>
+        <v>164392</v>
       </c>
       <c r="C7">
         <f t="shared" si="5"/>
-        <v>65076</v>
+        <v>97752</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="6"/>
-        <v>0.7517547607421875</v>
+        <v>0.627105712890625</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
@@ -26443,15 +26621,15 @@
         <v>91</v>
       </c>
       <c r="B8">
-        <v>154032</v>
+        <v>126912</v>
       </c>
       <c r="C8">
         <f t="shared" si="5"/>
-        <v>108112</v>
+        <v>135232</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="6"/>
-        <v>0.58758544921875</v>
+        <v>0.484130859375</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
@@ -26502,15 +26680,15 @@
         <v>92</v>
       </c>
       <c r="B9">
-        <v>103356</v>
+        <v>86504</v>
       </c>
       <c r="C9">
         <f t="shared" si="5"/>
-        <v>158788</v>
+        <v>175640</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="6"/>
-        <v>0.3942718505859375</v>
+        <v>0.329986572265625</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
@@ -26620,15 +26798,15 @@
         <v>94</v>
       </c>
       <c r="B11">
-        <v>97796</v>
+        <v>78900</v>
       </c>
       <c r="C11">
         <f t="shared" si="5"/>
-        <v>164348</v>
+        <v>183244</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="6"/>
-        <v>0.3730621337890625</v>
+        <v>0.3009796142578125</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
@@ -26679,15 +26857,15 @@
         <v>95</v>
       </c>
       <c r="B12">
-        <v>197248</v>
+        <v>164800</v>
       </c>
       <c r="C12">
         <f t="shared" si="5"/>
-        <v>64896</v>
+        <v>97344</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="6"/>
-        <v>0.75244140625</v>
+        <v>0.628662109375</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
@@ -26738,15 +26916,15 @@
         <v>96</v>
       </c>
       <c r="B13">
-        <v>138752</v>
+        <v>113988</v>
       </c>
       <c r="C13">
         <f t="shared" si="5"/>
-        <v>123392</v>
+        <v>148156</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="6"/>
-        <v>0.529296875</v>
+        <v>0.4348297119140625</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
@@ -26797,15 +26975,15 @@
         <v>97</v>
       </c>
       <c r="B14">
-        <v>164136</v>
+        <v>136888</v>
       </c>
       <c r="C14">
         <f t="shared" si="5"/>
-        <v>98008</v>
+        <v>125256</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="6"/>
-        <v>0.626129150390625</v>
+        <v>0.522186279296875</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
@@ -26856,15 +27034,15 @@
         <v>98</v>
       </c>
       <c r="B15">
-        <v>181388</v>
+        <v>151832</v>
       </c>
       <c r="C15">
         <f t="shared" si="5"/>
-        <v>80756</v>
+        <v>110312</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="6"/>
-        <v>0.6919403076171875</v>
+        <v>0.579193115234375</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
@@ -26915,15 +27093,15 @@
         <v>99</v>
       </c>
       <c r="B16">
-        <v>163660</v>
+        <v>135492</v>
       </c>
       <c r="C16">
         <f t="shared" si="5"/>
-        <v>98484</v>
+        <v>126652</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="6"/>
-        <v>0.6243133544921875</v>
+        <v>0.5168609619140625</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
@@ -26974,15 +27152,15 @@
         <v>100</v>
       </c>
       <c r="B17">
-        <v>197616</v>
+        <v>165864</v>
       </c>
       <c r="C17">
         <f t="shared" si="5"/>
-        <v>64528</v>
+        <v>96280</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="6"/>
-        <v>0.75384521484375</v>
+        <v>0.632720947265625</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
@@ -27033,15 +27211,15 @@
         <v>101</v>
       </c>
       <c r="B18">
-        <v>74292</v>
+        <v>60808</v>
       </c>
       <c r="C18">
         <f t="shared" si="5"/>
-        <v>187852</v>
+        <v>201336</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="6"/>
-        <v>0.2834014892578125</v>
+        <v>0.231964111328125</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
@@ -27151,15 +27329,15 @@
         <v>103</v>
       </c>
       <c r="B20">
-        <v>80580</v>
+        <v>64272</v>
       </c>
       <c r="C20">
         <f t="shared" si="5"/>
-        <v>181564</v>
+        <v>197872</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="6"/>
-        <v>0.3073883056640625</v>
+        <v>0.24517822265625</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
@@ -27210,15 +27388,15 @@
         <v>104</v>
       </c>
       <c r="B21">
-        <v>113980</v>
+        <v>92964</v>
       </c>
       <c r="C21">
         <f t="shared" si="5"/>
-        <v>148164</v>
+        <v>169180</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="6"/>
-        <v>0.4347991943359375</v>
+        <v>0.3546295166015625</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
@@ -27269,15 +27447,15 @@
         <v>105</v>
       </c>
       <c r="B22">
-        <v>151444</v>
+        <v>122872</v>
       </c>
       <c r="C22">
         <f t="shared" si="5"/>
-        <v>110700</v>
+        <v>139272</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" si="6"/>
-        <v>0.5777130126953125</v>
+        <v>0.468719482421875</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
@@ -27328,15 +27506,15 @@
         <v>106</v>
       </c>
       <c r="B23">
-        <v>168112</v>
+        <v>139744</v>
       </c>
       <c r="C23">
         <f t="shared" si="5"/>
-        <v>94032</v>
+        <v>122400</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" si="6"/>
-        <v>0.64129638671875</v>
+        <v>0.5330810546875</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
@@ -27387,15 +27565,15 @@
         <v>107</v>
       </c>
       <c r="B24">
-        <v>183988</v>
+        <v>152552</v>
       </c>
       <c r="C24">
         <f t="shared" si="5"/>
-        <v>78156</v>
+        <v>109592</v>
       </c>
       <c r="D24" s="1">
         <f t="shared" si="6"/>
-        <v>0.7018585205078125</v>
+        <v>0.581939697265625</v>
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
@@ -27446,15 +27624,15 @@
         <v>108</v>
       </c>
       <c r="B25">
-        <v>156788</v>
+        <v>129080</v>
       </c>
       <c r="C25">
         <f t="shared" si="5"/>
-        <v>105356</v>
+        <v>133064</v>
       </c>
       <c r="D25" s="1">
         <f t="shared" si="6"/>
-        <v>0.5980987548828125</v>
+        <v>0.492401123046875</v>
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
@@ -27505,15 +27683,15 @@
         <v>109</v>
       </c>
       <c r="B26">
-        <v>136976</v>
+        <v>112722</v>
       </c>
       <c r="C26">
         <f t="shared" si="5"/>
-        <v>125168</v>
+        <v>149422</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" si="6"/>
-        <v>0.52252197265625</v>
+        <v>0.43000030517578125</v>
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
@@ -27564,15 +27742,15 @@
         <v>110</v>
       </c>
       <c r="B27">
-        <v>68728</v>
+        <v>54224</v>
       </c>
       <c r="C27">
         <f t="shared" si="5"/>
-        <v>193416</v>
+        <v>207920</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" si="6"/>
-        <v>0.262176513671875</v>
+        <v>0.20684814453125</v>
       </c>
       <c r="E27">
         <f t="shared" si="0"/>
@@ -27682,15 +27860,15 @@
         <v>112</v>
       </c>
       <c r="B29">
-        <v>106076</v>
+        <v>85404</v>
       </c>
       <c r="C29">
         <f t="shared" si="5"/>
-        <v>156068</v>
+        <v>176740</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" si="6"/>
-        <v>0.4046478271484375</v>
+        <v>0.3257904052734375</v>
       </c>
       <c r="E29">
         <f t="shared" si="0"/>
@@ -27741,15 +27919,15 @@
         <v>113</v>
       </c>
       <c r="B30">
-        <v>142768</v>
+        <v>117112</v>
       </c>
       <c r="C30">
         <f t="shared" si="5"/>
-        <v>119376</v>
+        <v>145032</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" si="6"/>
-        <v>0.54461669921875</v>
+        <v>0.446746826171875</v>
       </c>
       <c r="E30">
         <f t="shared" si="0"/>
@@ -27800,15 +27978,15 @@
         <v>114</v>
       </c>
       <c r="B31">
-        <v>161720</v>
+        <v>134592</v>
       </c>
       <c r="C31">
         <f t="shared" si="5"/>
-        <v>100424</v>
+        <v>127552</v>
       </c>
       <c r="D31" s="1">
         <f t="shared" si="6"/>
-        <v>0.616912841796875</v>
+        <v>0.513427734375</v>
       </c>
       <c r="E31">
         <f t="shared" si="0"/>
@@ -27859,15 +28037,15 @@
         <v>115</v>
       </c>
       <c r="B32">
-        <v>110740</v>
+        <v>89492</v>
       </c>
       <c r="C32">
         <f t="shared" si="5"/>
-        <v>151404</v>
+        <v>172652</v>
       </c>
       <c r="D32" s="1">
         <f t="shared" si="6"/>
-        <v>0.4224395751953125</v>
+        <v>0.3413848876953125</v>
       </c>
       <c r="E32">
         <f t="shared" si="0"/>
@@ -27918,15 +28096,15 @@
         <v>116</v>
       </c>
       <c r="B33">
-        <v>168980</v>
+        <v>140220</v>
       </c>
       <c r="C33">
         <f t="shared" si="5"/>
-        <v>93164</v>
+        <v>121924</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" si="6"/>
-        <v>0.6446075439453125</v>
+        <v>0.5348968505859375</v>
       </c>
       <c r="E33">
         <f t="shared" si="0"/>
@@ -27977,15 +28155,15 @@
         <v>117</v>
       </c>
       <c r="B34">
-        <v>184264</v>
+        <v>152684</v>
       </c>
       <c r="C34">
         <f t="shared" si="5"/>
-        <v>77880</v>
+        <v>109460</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" si="6"/>
-        <v>0.702911376953125</v>
+        <v>0.5824432373046875</v>
       </c>
       <c r="E34">
         <f t="shared" si="0"/>
@@ -28036,15 +28214,15 @@
         <v>118</v>
       </c>
       <c r="B35">
-        <v>195892</v>
+        <v>162748</v>
       </c>
       <c r="C35">
         <f t="shared" si="5"/>
-        <v>66252</v>
+        <v>99396</v>
       </c>
       <c r="D35" s="1">
         <f t="shared" si="6"/>
-        <v>0.7472686767578125</v>
+        <v>0.6208343505859375</v>
       </c>
       <c r="E35">
         <f t="shared" si="0"/>
@@ -28095,15 +28273,15 @@
         <v>119</v>
       </c>
       <c r="B36">
-        <v>186336</v>
+        <v>153964</v>
       </c>
       <c r="C36">
         <f t="shared" si="5"/>
-        <v>75808</v>
+        <v>108180</v>
       </c>
       <c r="D36" s="1">
         <f t="shared" si="6"/>
-        <v>0.7108154296875</v>
+        <v>0.5873260498046875</v>
       </c>
       <c r="E36">
         <f t="shared" si="0"/>
@@ -28383,6 +28561,162 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0600-000000000000}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G2:G2</xm:f>
+              <xm:sqref>H2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G3:G3</xm:f>
+              <xm:sqref>H3</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G4:G4</xm:f>
+              <xm:sqref>H4</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G5:G5</xm:f>
+              <xm:sqref>H5</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G6:G6</xm:f>
+              <xm:sqref>H6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G7:G7</xm:f>
+              <xm:sqref>H7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G8:G8</xm:f>
+              <xm:sqref>H8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G9:G9</xm:f>
+              <xm:sqref>H9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G10:G10</xm:f>
+              <xm:sqref>H10</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G11:G11</xm:f>
+              <xm:sqref>H11</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G12:G12</xm:f>
+              <xm:sqref>H12</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G13:G13</xm:f>
+              <xm:sqref>H13</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G14:G14</xm:f>
+              <xm:sqref>H14</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G15:G15</xm:f>
+              <xm:sqref>H15</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G16:G16</xm:f>
+              <xm:sqref>H16</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G17:G17</xm:f>
+              <xm:sqref>H17</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G18:G18</xm:f>
+              <xm:sqref>H18</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G19:G19</xm:f>
+              <xm:sqref>H19</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G20:G20</xm:f>
+              <xm:sqref>H20</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G21:G21</xm:f>
+              <xm:sqref>H21</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G22:G22</xm:f>
+              <xm:sqref>H22</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G23:G23</xm:f>
+              <xm:sqref>H23</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G24:G24</xm:f>
+              <xm:sqref>H24</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G25:G25</xm:f>
+              <xm:sqref>H25</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G26:G26</xm:f>
+              <xm:sqref>H26</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G27:G27</xm:f>
+              <xm:sqref>H27</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G28:G28</xm:f>
+              <xm:sqref>H28</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G29:G29</xm:f>
+              <xm:sqref>H29</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G30:G30</xm:f>
+              <xm:sqref>H30</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G31:G31</xm:f>
+              <xm:sqref>H31</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G32:G32</xm:f>
+              <xm:sqref>H32</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G33:G33</xm:f>
+              <xm:sqref>H33</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G34:G34</xm:f>
+              <xm:sqref>H34</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G35:G35</xm:f>
+              <xm:sqref>H35</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G36:G36</xm:f>
+              <xm:sqref>H36</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!G37:G37</xm:f>
+              <xm:sqref>H37</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0600-000001000000}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
@@ -28539,162 +28873,6 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0600-000000000000}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G2:G2</xm:f>
-              <xm:sqref>H2</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G3:G3</xm:f>
-              <xm:sqref>H3</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G4:G4</xm:f>
-              <xm:sqref>H4</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G5:G5</xm:f>
-              <xm:sqref>H5</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G6:G6</xm:f>
-              <xm:sqref>H6</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G7:G7</xm:f>
-              <xm:sqref>H7</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G8:G8</xm:f>
-              <xm:sqref>H8</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G9:G9</xm:f>
-              <xm:sqref>H9</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G10:G10</xm:f>
-              <xm:sqref>H10</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G11:G11</xm:f>
-              <xm:sqref>H11</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G12:G12</xm:f>
-              <xm:sqref>H12</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G13:G13</xm:f>
-              <xm:sqref>H13</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G14:G14</xm:f>
-              <xm:sqref>H14</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G15:G15</xm:f>
-              <xm:sqref>H15</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G16:G16</xm:f>
-              <xm:sqref>H16</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G17:G17</xm:f>
-              <xm:sqref>H17</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G18:G18</xm:f>
-              <xm:sqref>H18</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G19:G19</xm:f>
-              <xm:sqref>H19</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G20:G20</xm:f>
-              <xm:sqref>H20</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G21:G21</xm:f>
-              <xm:sqref>H21</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G22:G22</xm:f>
-              <xm:sqref>H22</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G23:G23</xm:f>
-              <xm:sqref>H23</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G24:G24</xm:f>
-              <xm:sqref>H24</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G25:G25</xm:f>
-              <xm:sqref>H25</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G26:G26</xm:f>
-              <xm:sqref>H26</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G27:G27</xm:f>
-              <xm:sqref>H27</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G28:G28</xm:f>
-              <xm:sqref>H28</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G29:G29</xm:f>
-              <xm:sqref>H29</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G30:G30</xm:f>
-              <xm:sqref>H30</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G31:G31</xm:f>
-              <xm:sqref>H31</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G32:G32</xm:f>
-              <xm:sqref>H32</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G33:G33</xm:f>
-              <xm:sqref>H33</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G34:G34</xm:f>
-              <xm:sqref>H34</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G35:G35</xm:f>
-              <xm:sqref>H35</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G36:G36</xm:f>
-              <xm:sqref>H36</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!G37:G37</xm:f>
-              <xm:sqref>H37</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>
@@ -30699,7 +30877,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{D21CAF72-2AF7-4E10-80D4-49E1123EB21E}">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0700-000002000000}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -30710,8 +30888,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Doom2 Levels'!L2:L2</xm:f>
-              <xm:sqref>M2</xm:sqref>
+              <xm:f>'Doom2 Levels'!G2:G2</xm:f>
+              <xm:sqref>H2</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -30731,7 +30909,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0700-000002000000}">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{D21CAF72-2AF7-4E10-80D4-49E1123EB21E}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -30742,8 +30920,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Doom2 Levels'!G2:G2</xm:f>
-              <xm:sqref>H2</xm:sqref>
+              <xm:f>'Doom2 Levels'!L2:L2</xm:f>
+              <xm:sqref>M2</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -30757,8 +30935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E70020B-64A4-492D-9830-6A4BD6B3C292}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C41" sqref="A34:C41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30791,15 +30969,15 @@
         <v>85</v>
       </c>
       <c r="B2">
-        <v>194672</v>
+        <v>193056</v>
       </c>
       <c r="C2">
         <f>$E$2-B2</f>
-        <v>67472</v>
+        <v>69088</v>
       </c>
       <c r="D2" s="1">
         <f>1-(C2/$E$2)</f>
-        <v>0.74261474609375</v>
+        <v>0.7364501953125</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E10" si="0">256*1024</f>
@@ -30814,15 +30992,15 @@
         <v>86</v>
       </c>
       <c r="B3">
-        <v>193260</v>
+        <v>191532</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C10" si="1">$E$2-B3</f>
-        <v>68884</v>
+        <v>70612</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D10" si="2">1-(C3/$E$2)</f>
-        <v>0.7372283935546875</v>
+        <v>0.7306365966796875</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
@@ -30837,15 +31015,15 @@
         <v>87</v>
       </c>
       <c r="B4">
-        <v>159596</v>
+        <v>156940</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>102548</v>
+        <v>105204</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="2"/>
-        <v>0.6088104248046875</v>
+        <v>0.5986785888671875</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
@@ -30860,15 +31038,15 @@
         <v>88</v>
       </c>
       <c r="B5">
-        <v>334084</v>
+        <v>330172</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>-71940</v>
+        <v>-68028</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="2"/>
-        <v>1.2744293212890625</v>
+        <v>1.2595062255859375</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
@@ -30883,15 +31061,15 @@
         <v>89</v>
       </c>
       <c r="B6">
-        <v>249652</v>
+        <v>248084</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>12492</v>
+        <v>14060</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="2"/>
-        <v>0.9523468017578125</v>
+        <v>0.9463653564453125</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
@@ -30906,15 +31084,15 @@
         <v>90</v>
       </c>
       <c r="B7">
-        <v>384784</v>
+        <v>380064</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>-122640</v>
+        <v>-117920</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="2"/>
-        <v>1.46783447265625</v>
+        <v>1.4498291015625</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
@@ -30929,15 +31107,15 @@
         <v>91</v>
       </c>
       <c r="B8">
-        <v>416804</v>
+        <v>412212</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>-154660</v>
+        <v>-150068</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="2"/>
-        <v>1.5899810791015625</v>
+        <v>1.5724639892578125</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
@@ -30952,15 +31130,15 @@
         <v>92</v>
       </c>
       <c r="B9">
-        <v>196672</v>
+        <v>194480</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>65472</v>
+        <v>67664</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="2"/>
-        <v>0.750244140625</v>
+        <v>0.74188232421875</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Use id Zone allocator
</commit_message>
<xml_diff>
--- a/GBADoomMemory.xlsx
+++ b/GBADoomMemory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\GBADoom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3293F6B-57CB-4F3B-BC91-680564B85BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336A219D-219A-4F82-9902-37908716A251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6121,70 +6121,70 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>117480</c:v>
+                  <c:v>116520</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130088</c:v>
+                  <c:v>126952</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>128084</c:v>
+                  <c:v>127656</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>149536</c:v>
+                  <c:v>145288</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>134320</c:v>
+                  <c:v>135428</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>163368</c:v>
+                  <c:v>162480</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>98408</c:v>
+                  <c:v>98660</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>166324</c:v>
+                  <c:v>162952</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>203620</c:v>
+                  <c:v>201832</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>130528</c:v>
+                  <c:v>130184</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>148072</c:v>
+                  <c:v>143244</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>172084</c:v>
+                  <c:v>168366</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>156956</c:v>
+                  <c:v>151312</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>146208</c:v>
+                  <c:v>142376</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>162296</c:v>
+                  <c:v>159172</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>141304</c:v>
+                  <c:v>137944</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>165228</c:v>
+                  <c:v>161924</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>183092</c:v>
+                  <c:v>175588</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>150760</c:v>
+                  <c:v>148360</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>165728</c:v>
+                  <c:v>162380</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>112774</c:v>
+                  <c:v>114288</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>209108</c:v>
+                  <c:v>203392</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>257364</c:v>
@@ -14589,7 +14589,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14627,15 +14627,15 @@
         <v>121</v>
       </c>
       <c r="B2">
-        <v>117480</v>
+        <v>116520</v>
       </c>
       <c r="C2">
         <f>$E$2-B2</f>
-        <v>144664</v>
+        <v>145624</v>
       </c>
       <c r="D2" s="1">
         <f>1-(C2/$E$2)</f>
-        <v>0.448150634765625</v>
+        <v>0.444488525390625</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E33" si="0">256*1024</f>
@@ -14650,15 +14650,15 @@
         <v>122</v>
       </c>
       <c r="B3">
-        <v>130088</v>
+        <v>126952</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C33" si="1">$E$2-B3</f>
-        <v>132056</v>
+        <v>135192</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D33" si="2">1-(C3/$E$2)</f>
-        <v>0.496246337890625</v>
+        <v>0.484283447265625</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
@@ -14673,15 +14673,15 @@
         <v>123</v>
       </c>
       <c r="B4">
-        <v>128084</v>
+        <v>127656</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>134060</v>
+        <v>134488</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="2"/>
-        <v>0.4886016845703125</v>
+        <v>0.486968994140625</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
@@ -14696,15 +14696,15 @@
         <v>124</v>
       </c>
       <c r="B5">
-        <v>149536</v>
+        <v>145288</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>112608</v>
+        <v>116856</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="2"/>
-        <v>0.5704345703125</v>
+        <v>0.554229736328125</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
@@ -14719,15 +14719,15 @@
         <v>125</v>
       </c>
       <c r="B6">
-        <v>134320</v>
+        <v>135428</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>127824</v>
+        <v>126716</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="2"/>
-        <v>0.51239013671875</v>
+        <v>0.5166168212890625</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
@@ -14742,15 +14742,15 @@
         <v>126</v>
       </c>
       <c r="B7">
-        <v>163368</v>
+        <v>162480</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>98776</v>
+        <v>99664</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="2"/>
-        <v>0.623199462890625</v>
+        <v>0.61981201171875</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
@@ -14765,15 +14765,15 @@
         <v>127</v>
       </c>
       <c r="B8">
-        <v>98408</v>
+        <v>98660</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>163736</v>
+        <v>163484</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="2"/>
-        <v>0.375396728515625</v>
+        <v>0.3763580322265625</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
@@ -14788,15 +14788,15 @@
         <v>128</v>
       </c>
       <c r="B9">
-        <v>166324</v>
+        <v>162952</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>95820</v>
+        <v>99192</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="2"/>
-        <v>0.6344757080078125</v>
+        <v>0.621612548828125</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
@@ -14811,15 +14811,15 @@
         <v>129</v>
       </c>
       <c r="B10">
-        <v>203620</v>
+        <v>201832</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>58524</v>
+        <v>60312</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="2"/>
-        <v>0.7767486572265625</v>
+        <v>0.769927978515625</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
@@ -14834,15 +14834,15 @@
         <v>130</v>
       </c>
       <c r="B11">
-        <v>130528</v>
+        <v>130184</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>131616</v>
+        <v>131960</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="2"/>
-        <v>0.4979248046875</v>
+        <v>0.496612548828125</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
@@ -14857,15 +14857,15 @@
         <v>131</v>
       </c>
       <c r="B12">
-        <v>148072</v>
+        <v>143244</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>114072</v>
+        <v>118900</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="2"/>
-        <v>0.564849853515625</v>
+        <v>0.5464324951171875</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
@@ -14880,15 +14880,15 @@
         <v>132</v>
       </c>
       <c r="B13">
-        <v>172084</v>
+        <v>168366</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>90060</v>
+        <v>93778</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="2"/>
-        <v>0.6564483642578125</v>
+        <v>0.64226531982421875</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
@@ -14903,15 +14903,15 @@
         <v>133</v>
       </c>
       <c r="B14">
-        <v>156956</v>
+        <v>151312</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>105188</v>
+        <v>110832</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="2"/>
-        <v>0.5987396240234375</v>
+        <v>0.57720947265625</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
@@ -14926,15 +14926,15 @@
         <v>134</v>
       </c>
       <c r="B15">
-        <v>146208</v>
+        <v>142376</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>115936</v>
+        <v>119768</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="2"/>
-        <v>0.5577392578125</v>
+        <v>0.543121337890625</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
@@ -14949,15 +14949,15 @@
         <v>135</v>
       </c>
       <c r="B16">
-        <v>162296</v>
+        <v>159172</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>99848</v>
+        <v>102972</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="2"/>
-        <v>0.619110107421875</v>
+        <v>0.6071929931640625</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
@@ -14972,15 +14972,15 @@
         <v>136</v>
       </c>
       <c r="B17">
-        <v>141304</v>
+        <v>137944</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>120840</v>
+        <v>124200</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="2"/>
-        <v>0.539031982421875</v>
+        <v>0.526214599609375</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
@@ -14995,15 +14995,15 @@
         <v>137</v>
       </c>
       <c r="B18">
-        <v>165228</v>
+        <v>161924</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>96916</v>
+        <v>100220</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="2"/>
-        <v>0.6302947998046875</v>
+        <v>0.6176910400390625</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
@@ -15018,15 +15018,15 @@
         <v>138</v>
       </c>
       <c r="B19">
-        <v>183092</v>
+        <v>175588</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>79052</v>
+        <v>86556</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="2"/>
-        <v>0.6984405517578125</v>
+        <v>0.6698150634765625</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
@@ -15041,15 +15041,15 @@
         <v>139</v>
       </c>
       <c r="B20">
-        <v>150760</v>
+        <v>148360</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>111384</v>
+        <v>113784</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="2"/>
-        <v>0.575103759765625</v>
+        <v>0.565948486328125</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
@@ -15064,15 +15064,15 @@
         <v>140</v>
       </c>
       <c r="B21">
-        <v>165728</v>
+        <v>162380</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>96416</v>
+        <v>99764</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="2"/>
-        <v>0.6322021484375</v>
+        <v>0.6194305419921875</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
@@ -15085,15 +15085,15 @@
         <v>141</v>
       </c>
       <c r="B22">
-        <v>112774</v>
+        <v>114288</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>149370</v>
+        <v>147856</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" si="2"/>
-        <v>0.43019866943359375</v>
+        <v>0.43597412109375</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
@@ -15106,15 +15106,15 @@
         <v>142</v>
       </c>
       <c r="B23">
-        <v>209108</v>
+        <v>203392</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>53036</v>
+        <v>58752</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" si="2"/>
-        <v>0.7976837158203125</v>
+        <v>0.77587890625</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
@@ -20995,7 +20995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C55" sqref="C55:C57"/>
     </sheetView>
   </sheetViews>
@@ -26188,8 +26188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28561,6 +28561,162 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0600-000001000000}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J2:J2</xm:f>
+              <xm:sqref>K2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J3:J3</xm:f>
+              <xm:sqref>K3</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J4:J4</xm:f>
+              <xm:sqref>K4</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J5:J5</xm:f>
+              <xm:sqref>K5</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J6:J6</xm:f>
+              <xm:sqref>K6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J7:J7</xm:f>
+              <xm:sqref>K7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J8:J8</xm:f>
+              <xm:sqref>K8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J9:J9</xm:f>
+              <xm:sqref>K9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J10:J10</xm:f>
+              <xm:sqref>K10</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J11:J11</xm:f>
+              <xm:sqref>K11</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J12:J12</xm:f>
+              <xm:sqref>K12</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J13:J13</xm:f>
+              <xm:sqref>K13</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J14:J14</xm:f>
+              <xm:sqref>K14</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J15:J15</xm:f>
+              <xm:sqref>K15</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J16:J16</xm:f>
+              <xm:sqref>K16</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J17:J17</xm:f>
+              <xm:sqref>K17</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J18:J18</xm:f>
+              <xm:sqref>K18</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J19:J19</xm:f>
+              <xm:sqref>K19</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J20:J20</xm:f>
+              <xm:sqref>K20</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J21:J21</xm:f>
+              <xm:sqref>K21</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J22:J22</xm:f>
+              <xm:sqref>K22</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J23:J23</xm:f>
+              <xm:sqref>K23</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J24:J24</xm:f>
+              <xm:sqref>K24</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J25:J25</xm:f>
+              <xm:sqref>K25</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J26:J26</xm:f>
+              <xm:sqref>K26</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J27:J27</xm:f>
+              <xm:sqref>K27</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J28:J28</xm:f>
+              <xm:sqref>K28</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J29:J29</xm:f>
+              <xm:sqref>K29</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J30:J30</xm:f>
+              <xm:sqref>K30</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J31:J31</xm:f>
+              <xm:sqref>K31</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J32:J32</xm:f>
+              <xm:sqref>K32</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J33:J33</xm:f>
+              <xm:sqref>K33</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J34:J34</xm:f>
+              <xm:sqref>K34</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J35:J35</xm:f>
+              <xm:sqref>K35</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J36:J36</xm:f>
+              <xm:sqref>K36</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J37:J37</xm:f>
+              <xm:sqref>K37</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0600-000000000000}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
@@ -28717,162 +28873,6 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0600-000001000000}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J2:J2</xm:f>
-              <xm:sqref>K2</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J3:J3</xm:f>
-              <xm:sqref>K3</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J4:J4</xm:f>
-              <xm:sqref>K4</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J5:J5</xm:f>
-              <xm:sqref>K5</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J6:J6</xm:f>
-              <xm:sqref>K6</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J7:J7</xm:f>
-              <xm:sqref>K7</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J8:J8</xm:f>
-              <xm:sqref>K8</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J9:J9</xm:f>
-              <xm:sqref>K9</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J10:J10</xm:f>
-              <xm:sqref>K10</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J11:J11</xm:f>
-              <xm:sqref>K11</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J12:J12</xm:f>
-              <xm:sqref>K12</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J13:J13</xm:f>
-              <xm:sqref>K13</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J14:J14</xm:f>
-              <xm:sqref>K14</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J15:J15</xm:f>
-              <xm:sqref>K15</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J16:J16</xm:f>
-              <xm:sqref>K16</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J17:J17</xm:f>
-              <xm:sqref>K17</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J18:J18</xm:f>
-              <xm:sqref>K18</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J19:J19</xm:f>
-              <xm:sqref>K19</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J20:J20</xm:f>
-              <xm:sqref>K20</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J21:J21</xm:f>
-              <xm:sqref>K21</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J22:J22</xm:f>
-              <xm:sqref>K22</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J23:J23</xm:f>
-              <xm:sqref>K23</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J24:J24</xm:f>
-              <xm:sqref>K24</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J25:J25</xm:f>
-              <xm:sqref>K25</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J26:J26</xm:f>
-              <xm:sqref>K26</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J27:J27</xm:f>
-              <xm:sqref>K27</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J28:J28</xm:f>
-              <xm:sqref>K28</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J29:J29</xm:f>
-              <xm:sqref>K29</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J30:J30</xm:f>
-              <xm:sqref>K30</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J31:J31</xm:f>
-              <xm:sqref>K31</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J32:J32</xm:f>
-              <xm:sqref>K32</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J33:J33</xm:f>
-              <xm:sqref>K33</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J34:J34</xm:f>
-              <xm:sqref>K34</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J35:J35</xm:f>
-              <xm:sqref>K35</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J36:J36</xm:f>
-              <xm:sqref>K36</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J37:J37</xm:f>
-              <xm:sqref>K37</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>
@@ -30877,7 +30877,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0700-000002000000}">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{D21CAF72-2AF7-4E10-80D4-49E1123EB21E}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -30888,8 +30888,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Doom2 Levels'!G2:G2</xm:f>
-              <xm:sqref>H2</xm:sqref>
+              <xm:f>'Doom2 Levels'!L2:L2</xm:f>
+              <xm:sqref>M2</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -30909,7 +30909,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{D21CAF72-2AF7-4E10-80D4-49E1123EB21E}">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0700-000002000000}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -30920,8 +30920,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Doom2 Levels'!L2:L2</xm:f>
-              <xm:sqref>M2</xm:sqref>
+              <xm:f>'Doom2 Levels'!G2:G2</xm:f>
+              <xm:sqref>H2</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>

<commit_message>
Revert testing changes to menu
</commit_message>
<xml_diff>
--- a/GBADoomMemory.xlsx
+++ b/GBADoomMemory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\GBADoom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FF63A8-8BD6-4EAE-84A8-DDC1CE777006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B91086-424D-4523-AA75-619A1B14856F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Globals" sheetId="1" r:id="rId1"/>
@@ -4673,7 +4673,7 @@
                   <c:v>86504</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>129824</c:v>
+                  <c:v>106704</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>78900</c:v>
@@ -4700,7 +4700,7 @@
                   <c:v>60808</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>70880</c:v>
+                  <c:v>58040</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>64272</c:v>
@@ -4727,7 +4727,7 @@
                   <c:v>54224</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>119224</c:v>
+                  <c:v>99744</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>85404</c:v>
@@ -4754,7 +4754,7 @@
                   <c:v>153964</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>198756</c:v>
+                  <c:v>159232</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5518,10 +5518,10 @@
                   <c:v>82832</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>143968</c:v>
+                  <c:v>121900</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>92084</c:v>
+                  <c:v>77308</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6102,28 +6102,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>193056</c:v>
+                  <c:v>182784</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>191532</c:v>
+                  <c:v>183848</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>156940</c:v>
+                  <c:v>151756</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>330172</c:v>
+                  <c:v>305792</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>248084</c:v>
+                  <c:v>236420</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>380064</c:v>
+                  <c:v>352460</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>412212</c:v>
+                  <c:v>382848</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>194480</c:v>
+                  <c:v>184836</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>231068</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -27619,8 +27622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28170,15 +28173,15 @@
         <v>93</v>
       </c>
       <c r="B10">
-        <v>129824</v>
+        <v>106704</v>
       </c>
       <c r="C10">
         <f t="shared" si="5"/>
-        <v>132320</v>
+        <v>155440</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="6"/>
-        <v>0.4952392578125</v>
+        <v>0.40704345703125</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
@@ -28701,15 +28704,15 @@
         <v>102</v>
       </c>
       <c r="B19">
-        <v>70880</v>
+        <v>58040</v>
       </c>
       <c r="C19">
         <f t="shared" si="5"/>
-        <v>191264</v>
+        <v>204104</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="6"/>
-        <v>0.2703857421875</v>
+        <v>0.221405029296875</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
@@ -29232,15 +29235,15 @@
         <v>111</v>
       </c>
       <c r="B28">
-        <v>119224</v>
+        <v>99744</v>
       </c>
       <c r="C28">
         <f t="shared" si="5"/>
-        <v>142920</v>
+        <v>162400</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" si="6"/>
-        <v>0.454803466796875</v>
+        <v>0.3804931640625</v>
       </c>
       <c r="E28">
         <f t="shared" si="0"/>
@@ -29763,15 +29766,15 @@
         <v>120</v>
       </c>
       <c r="B37">
-        <v>198756</v>
+        <v>159232</v>
       </c>
       <c r="C37">
         <f t="shared" si="5"/>
-        <v>63388</v>
+        <v>102912</v>
       </c>
       <c r="D37" s="1">
         <f t="shared" si="6"/>
-        <v>0.7581939697265625</v>
+        <v>0.607421875</v>
       </c>
       <c r="E37">
         <f t="shared" si="0"/>
@@ -30314,8 +30317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32163,15 +32166,15 @@
         <v>151</v>
       </c>
       <c r="B32">
-        <v>143968</v>
+        <v>121900</v>
       </c>
       <c r="C32">
         <f t="shared" si="6"/>
-        <v>118176</v>
+        <v>140244</v>
       </c>
       <c r="D32" s="1">
         <f t="shared" si="7"/>
-        <v>0.5491943359375</v>
+        <v>0.4650115966796875</v>
       </c>
       <c r="E32">
         <f t="shared" si="0"/>
@@ -32205,15 +32208,15 @@
         <v>152</v>
       </c>
       <c r="B33">
-        <v>92084</v>
+        <v>77308</v>
       </c>
       <c r="C33">
         <f t="shared" si="6"/>
-        <v>170060</v>
+        <v>184836</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" si="7"/>
-        <v>0.3512725830078125</v>
+        <v>0.2949066162109375</v>
       </c>
       <c r="E33">
         <f t="shared" si="0"/>
@@ -32366,8 +32369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E70020B-64A4-492D-9830-6A4BD6B3C292}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32400,15 +32403,15 @@
         <v>85</v>
       </c>
       <c r="B2">
-        <v>193056</v>
+        <v>182784</v>
       </c>
       <c r="C2">
         <f>$E$2-B2</f>
-        <v>69088</v>
+        <v>79360</v>
       </c>
       <c r="D2" s="1">
         <f>1-(C2/$E$2)</f>
-        <v>0.7364501953125</v>
+        <v>0.697265625</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E10" si="0">256*1024</f>
@@ -32423,15 +32426,15 @@
         <v>86</v>
       </c>
       <c r="B3">
-        <v>191532</v>
+        <v>183848</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C10" si="1">$E$2-B3</f>
-        <v>70612</v>
+        <v>78296</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D10" si="2">1-(C3/$E$2)</f>
-        <v>0.7306365966796875</v>
+        <v>0.701324462890625</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
@@ -32446,15 +32449,15 @@
         <v>87</v>
       </c>
       <c r="B4">
-        <v>156940</v>
+        <v>151756</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>105204</v>
+        <v>110388</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="2"/>
-        <v>0.5986785888671875</v>
+        <v>0.5789031982421875</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
@@ -32469,15 +32472,15 @@
         <v>88</v>
       </c>
       <c r="B5">
-        <v>330172</v>
+        <v>305792</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>-68028</v>
+        <v>-43648</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="2"/>
-        <v>1.2595062255859375</v>
+        <v>1.16650390625</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
@@ -32492,15 +32495,15 @@
         <v>89</v>
       </c>
       <c r="B6">
-        <v>248084</v>
+        <v>236420</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>14060</v>
+        <v>25724</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="2"/>
-        <v>0.9463653564453125</v>
+        <v>0.9018707275390625</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
@@ -32515,15 +32518,15 @@
         <v>90</v>
       </c>
       <c r="B7">
-        <v>380064</v>
+        <v>352460</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>-117920</v>
+        <v>-90316</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="2"/>
-        <v>1.4498291015625</v>
+        <v>1.3445281982421875</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
@@ -32538,15 +32541,15 @@
         <v>91</v>
       </c>
       <c r="B8">
-        <v>412212</v>
+        <v>382848</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>-150068</v>
+        <v>-120704</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="2"/>
-        <v>1.5724639892578125</v>
+        <v>1.46044921875</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
@@ -32561,15 +32564,15 @@
         <v>92</v>
       </c>
       <c r="B9">
-        <v>194480</v>
+        <v>184836</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>67664</v>
+        <v>77308</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="2"/>
-        <v>0.74188232421875</v>
+        <v>0.7050933837890625</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
@@ -32583,13 +32586,16 @@
       <c r="A10" t="s">
         <v>93</v>
       </c>
+      <c r="B10">
+        <v>231068</v>
+      </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>262144</v>
+        <v>31076</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.8814544677734375</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Code tidy. Fix some warnings.
</commit_message>
<xml_diff>
--- a/GBADoomMemory.xlsx
+++ b/GBADoomMemory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zak\Documents\GitProjects\GBADoom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD551412-F650-42A3-B99D-D8C436819EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652537E6-6E4F-4EEE-AAFF-E2F6FA05A69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26148,8 +26148,8 @@
   <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28108,14 +28108,14 @@
       </c>
       <c r="F69" s="2">
         <f t="shared" ref="F69" si="155">H69-E69</f>
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="G69" s="1">
         <f t="shared" ref="G69" si="156">1-(F69/H69)</f>
-        <v>0.96566877231529802</v>
+        <v>0.9656982421875</v>
       </c>
       <c r="H69">
-        <v>32769</v>
+        <v>32768</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -28137,14 +28137,14 @@
       </c>
       <c r="F70" s="2">
         <f t="shared" ref="F70" si="158">H70-E70</f>
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="G70" s="1">
         <f t="shared" ref="G70" si="159">1-(F70/H70)</f>
-        <v>0.96417454989319495</v>
+        <v>0.9642333984375</v>
       </c>
       <c r="H70">
-        <v>32770</v>
+        <v>32768</v>
       </c>
     </row>
   </sheetData>
@@ -30528,6 +30528,162 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0600-000001000000}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J2:J2</xm:f>
+              <xm:sqref>K2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J3:J3</xm:f>
+              <xm:sqref>K3</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J4:J4</xm:f>
+              <xm:sqref>K4</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J5:J5</xm:f>
+              <xm:sqref>K5</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J6:J6</xm:f>
+              <xm:sqref>K6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J7:J7</xm:f>
+              <xm:sqref>K7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J8:J8</xm:f>
+              <xm:sqref>K8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J9:J9</xm:f>
+              <xm:sqref>K9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J10:J10</xm:f>
+              <xm:sqref>K10</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J11:J11</xm:f>
+              <xm:sqref>K11</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J12:J12</xm:f>
+              <xm:sqref>K12</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J13:J13</xm:f>
+              <xm:sqref>K13</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J14:J14</xm:f>
+              <xm:sqref>K14</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J15:J15</xm:f>
+              <xm:sqref>K15</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J16:J16</xm:f>
+              <xm:sqref>K16</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J17:J17</xm:f>
+              <xm:sqref>K17</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J18:J18</xm:f>
+              <xm:sqref>K18</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J19:J19</xm:f>
+              <xm:sqref>K19</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J20:J20</xm:f>
+              <xm:sqref>K20</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J21:J21</xm:f>
+              <xm:sqref>K21</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J22:J22</xm:f>
+              <xm:sqref>K22</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J23:J23</xm:f>
+              <xm:sqref>K23</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J24:J24</xm:f>
+              <xm:sqref>K24</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J25:J25</xm:f>
+              <xm:sqref>K25</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J26:J26</xm:f>
+              <xm:sqref>K26</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J27:J27</xm:f>
+              <xm:sqref>K27</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J28:J28</xm:f>
+              <xm:sqref>K28</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J29:J29</xm:f>
+              <xm:sqref>K29</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J30:J30</xm:f>
+              <xm:sqref>K30</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J31:J31</xm:f>
+              <xm:sqref>K31</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J32:J32</xm:f>
+              <xm:sqref>K32</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J33:J33</xm:f>
+              <xm:sqref>K33</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J34:J34</xm:f>
+              <xm:sqref>K34</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J35:J35</xm:f>
+              <xm:sqref>K35</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J36:J36</xm:f>
+              <xm:sqref>K36</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Doom Levels'!J37:J37</xm:f>
+              <xm:sqref>K37</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0600-000000000000}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
@@ -30684,162 +30840,6 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0600-000001000000}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J2:J2</xm:f>
-              <xm:sqref>K2</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J3:J3</xm:f>
-              <xm:sqref>K3</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J4:J4</xm:f>
-              <xm:sqref>K4</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J5:J5</xm:f>
-              <xm:sqref>K5</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J6:J6</xm:f>
-              <xm:sqref>K6</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J7:J7</xm:f>
-              <xm:sqref>K7</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J8:J8</xm:f>
-              <xm:sqref>K8</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J9:J9</xm:f>
-              <xm:sqref>K9</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J10:J10</xm:f>
-              <xm:sqref>K10</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J11:J11</xm:f>
-              <xm:sqref>K11</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J12:J12</xm:f>
-              <xm:sqref>K12</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J13:J13</xm:f>
-              <xm:sqref>K13</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J14:J14</xm:f>
-              <xm:sqref>K14</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J15:J15</xm:f>
-              <xm:sqref>K15</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J16:J16</xm:f>
-              <xm:sqref>K16</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J17:J17</xm:f>
-              <xm:sqref>K17</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J18:J18</xm:f>
-              <xm:sqref>K18</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J19:J19</xm:f>
-              <xm:sqref>K19</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J20:J20</xm:f>
-              <xm:sqref>K20</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J21:J21</xm:f>
-              <xm:sqref>K21</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J22:J22</xm:f>
-              <xm:sqref>K22</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J23:J23</xm:f>
-              <xm:sqref>K23</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J24:J24</xm:f>
-              <xm:sqref>K24</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J25:J25</xm:f>
-              <xm:sqref>K25</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J26:J26</xm:f>
-              <xm:sqref>K26</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J27:J27</xm:f>
-              <xm:sqref>K27</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J28:J28</xm:f>
-              <xm:sqref>K28</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J29:J29</xm:f>
-              <xm:sqref>K29</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J30:J30</xm:f>
-              <xm:sqref>K30</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J31:J31</xm:f>
-              <xm:sqref>K31</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J32:J32</xm:f>
-              <xm:sqref>K32</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J33:J33</xm:f>
-              <xm:sqref>K33</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J34:J34</xm:f>
-              <xm:sqref>K34</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J35:J35</xm:f>
-              <xm:sqref>K35</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J36:J36</xm:f>
-              <xm:sqref>K36</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>'Doom Levels'!J37:J37</xm:f>
-              <xm:sqref>K37</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>
@@ -32844,7 +32844,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0700-000002000000}">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{D21CAF72-2AF7-4E10-80D4-49E1123EB21E}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -32855,8 +32855,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Doom2 Levels'!G2:G2</xm:f>
-              <xm:sqref>H2</xm:sqref>
+              <xm:f>'Doom2 Levels'!L2:L2</xm:f>
+              <xm:sqref>M2</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -32876,7 +32876,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{D21CAF72-2AF7-4E10-80D4-49E1123EB21E}">
+        <x14:sparklineGroup displayEmptyCellsAs="span" xr2:uid="{00000000-0003-0000-0700-000002000000}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -32887,8 +32887,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Doom2 Levels'!L2:L2</xm:f>
-              <xm:sqref>M2</xm:sqref>
+              <xm:f>'Doom2 Levels'!G2:G2</xm:f>
+              <xm:sqref>H2</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>